<commit_message>
Separação dos script FAT e RGPS (valores verificados)
</commit_message>
<xml_diff>
--- a/Teste R/FundosBI_R_SET_2025.xlsx
+++ b/Teste R/FundosBI_R_SET_2025.xlsx
@@ -461,7 +461,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="O7" sqref="O7:O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,46 +765,46 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>61780275142.580002</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>13867662856.940001</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>220268388.00999999</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>1658635.37</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>75869865022.899994</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>0</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="2">
         <v>75869865022.899994</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="2">
         <v>17049653001</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="2">
         <v>39990987157.209999</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
         <v>19579779094.220001</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>309684793.76999998</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="2">
         <v>76930104046.199997</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="2">
         <v>15989413977.700001</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="2">
         <v>-1060239023.3</v>
       </c>
     </row>
@@ -812,46 +812,46 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>75040272019.330002</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>15309766695.15</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>417797366.69</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="2">
         <v>301198866.57999998</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2">
         <v>91069034947.75</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="2">
         <v>9812204841</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="2">
         <v>81256830106.75</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="2">
         <v>20773345591.990002</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="2">
         <v>35736444942.089996</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <v>10158254487.969999</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>288227679.67000002</v>
       </c>
-      <c r="M8" s="1">
+      <c r="M8" s="2">
         <v>66956272701.720001</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="2">
         <v>35073902997.019997</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="2">
         <v>14300557405.030001</v>
       </c>
     </row>
@@ -859,46 +859,46 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>79018001998.050003</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>27100123081.02</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>293329748.29000002</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="2">
         <v>2352298527.9000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>108763753355.25999</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="2">
         <v>11192064717.700001</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>97571688637.559998</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="2">
         <v>22181668092.049999</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="2">
         <v>40680325821.559998</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <v>23564057523.110001</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>283435904.25999999</v>
       </c>
-      <c r="M9" s="1">
+      <c r="M9" s="2">
         <v>86709487340.979996</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="2">
         <v>33043869388.630001</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="2">
         <v>10862201296.58</v>
       </c>
     </row>
@@ -906,46 +906,46 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>83458886167.919998</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>27136201341.330002</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>663267291.26999998</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="2">
         <v>7495294474.0100002</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2">
         <v>118753649274.53</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="2">
         <v>22402550288.700001</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="2">
         <v>96351098985.830002</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="2">
         <v>23274204999.619999</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="2">
         <v>47775164661.809998</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>25020000812</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="2">
         <v>419796121.14999998</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="2">
         <v>96489166594.580002</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="2">
         <v>23136137390.869999</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="2">
         <v>-138067608.75</v>
       </c>
     </row>
@@ -953,46 +953,46 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>101923163946.50999</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>26345134572.240002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>603834237.05999994</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>729664179.16999996</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>129601796934.98</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>21499580680.07</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>108102216254.91</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="2">
         <v>28361807348.040001</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="2">
         <v>52350535752.720001</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <v>28291337053</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>508369173.05000001</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>109512049326.81</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="2">
         <v>26951974276.139999</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="2">
         <v>-1409833071.8999901</v>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,22 +1209,22 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>405787232623.15002</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>663505022341.45996</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>25771778971831</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="2">
         <v>640512546841.23999</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>3125537377.2399998</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="2">
         <v>19866938122.98</v>
       </c>
     </row>

</xml_diff>